<commit_message>
added movement rebuild framework
</commit_message>
<xml_diff>
--- a/Documentation/Gant Chart.xlsx
+++ b/Documentation/Gant Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hopet\OneDrive\Documents\Github\mgp-team-22\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A4A7A6-9ECE-4758-89A4-B2414416A04D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A888A9-C656-4277-B3DE-DB8335E11F61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{847660BB-F542-4C06-8F9C-28E685A168BD}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{847660BB-F542-4C06-8F9C-28E685A168BD}"/>
   </bookViews>
   <sheets>
     <sheet name="GANT" sheetId="2" r:id="rId1"/>
@@ -783,17 +783,8 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -805,12 +796,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -850,9 +835,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -912,12 +894,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -936,13 +912,37 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1262,61 +1262,63 @@
   <dimension ref="A1:EC115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="45" customWidth="1"/>
-    <col min="2" max="10" width="8.7109375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="9" customWidth="1"/>
+    <col min="6" max="10" width="8.7109375" style="9" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" style="15" customWidth="1"/>
     <col min="12" max="13" width="8.7109375" style="9" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="10" customWidth="1"/>
-    <col min="15" max="15" width="1" style="100" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="45" customWidth="1"/>
+    <col min="15" max="15" width="1" style="92" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" style="40" customWidth="1"/>
     <col min="17" max="21" width="9.140625" style="9"/>
-    <col min="22" max="22" width="9.140625" style="61"/>
+    <col min="22" max="22" width="9.140625" style="56"/>
     <col min="23" max="132" width="9.140625" style="9"/>
     <col min="133" max="133" width="9.140625" style="16"/>
     <col min="134" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:133" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="87" t="s">
+      <c r="G1" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="58" t="s">
+      <c r="M1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="O1" s="98"/>
-      <c r="P1" s="105" t="s">
+      <c r="O1" s="90"/>
+      <c r="P1" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="U1" s="83" t="s">
+      <c r="U1" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="V1" s="59" t="s">
+      <c r="V1" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="Y1" s="86" t="s">
+      <c r="Y1" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="Z1" s="55" t="s">
+      <c r="Z1" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" s="58" t="s">
+      <c r="AB1" s="53" t="s">
         <v>108</v>
       </c>
       <c r="AC1" s="10"/>
@@ -1425,7 +1427,7 @@
       <c r="EB1" s="16"/>
     </row>
     <row r="2" spans="1:133" s="11" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94"/>
+      <c r="A2" s="98"/>
       <c r="B2" s="11" t="s">
         <v>64</v>
       </c>
@@ -1438,10 +1440,10 @@
       <c r="E2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="88" t="s">
+      <c r="G2" s="82" t="s">
         <v>70</v>
       </c>
       <c r="H2" s="11" t="s">
@@ -1450,21 +1452,21 @@
       <c r="I2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="78" t="s">
         <v>73</v>
       </c>
       <c r="K2" s="12"/>
       <c r="L2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="56" t="s">
+      <c r="M2" s="51" t="s">
         <v>62</v>
       </c>
       <c r="N2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="99"/>
-      <c r="P2" s="105"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="97"/>
       <c r="Q2" s="11" t="s">
         <v>64</v>
       </c>
@@ -1477,10 +1479,10 @@
       <c r="T2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="U2" s="84" t="s">
+      <c r="U2" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="V2" s="60" t="s">
+      <c r="V2" s="55" t="s">
         <v>70</v>
       </c>
       <c r="W2" s="11" t="s">
@@ -1489,14 +1491,14 @@
       <c r="X2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="Y2" s="84" t="s">
+      <c r="Y2" s="78" t="s">
         <v>73</v>
       </c>
       <c r="Z2" s="12"/>
       <c r="AA2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="AB2" s="56" t="s">
+      <c r="AB2" s="51" t="s">
         <v>62</v>
       </c>
       <c r="AC2" s="13" t="s">
@@ -1608,7 +1610,7 @@
       <c r="EC2" s="17"/>
     </row>
     <row r="3" spans="1:133" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="95"/>
+      <c r="A3" s="99"/>
       <c r="B3" s="9" t="s">
         <v>43</v>
       </c>
@@ -1621,10 +1623,10 @@
       <c r="E3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -1633,7 +1635,7 @@
       <c r="I3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="85" t="s">
+      <c r="J3" s="79" t="s">
         <v>51</v>
       </c>
       <c r="K3" s="14" t="s">
@@ -1642,13 +1644,13 @@
       <c r="L3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="57" t="s">
+      <c r="M3" s="52" t="s">
         <v>53</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="105"/>
+      <c r="P3" s="97"/>
       <c r="Q3" s="9" t="s">
         <v>43</v>
       </c>
@@ -1661,10 +1663,10 @@
       <c r="T3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="85" t="s">
+      <c r="U3" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="61" t="s">
+      <c r="V3" s="56" t="s">
         <v>48</v>
       </c>
       <c r="W3" s="9" t="s">
@@ -1673,7 +1675,7 @@
       <c r="X3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="Y3" s="85" t="s">
+      <c r="Y3" s="79" t="s">
         <v>51</v>
       </c>
       <c r="Z3" s="14" t="s">
@@ -1682,7 +1684,7 @@
       <c r="AA3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AB3" s="57" t="s">
+      <c r="AB3" s="52" t="s">
         <v>53</v>
       </c>
       <c r="AC3" s="10" t="s">
@@ -1793,42 +1795,42 @@
       <c r="EB3" s="16"/>
     </row>
     <row r="4" spans="1:133" s="22" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
       <c r="K4" s="24"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="43"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="38"/>
       <c r="N4" s="20"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="79" t="s">
+      <c r="O4" s="93"/>
+      <c r="P4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="62" t="s">
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
-      <c r="Y4" s="48"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="43"/>
       <c r="Z4" s="15"/>
-      <c r="AA4" s="32" t="s">
+      <c r="AA4" s="101" t="s">
         <v>107</v>
       </c>
-      <c r="AB4" s="33" t="s">
+      <c r="AB4" s="102" t="s">
         <v>106</v>
       </c>
       <c r="AC4" s="10"/>
@@ -1938,36 +1940,36 @@
       <c r="EC4" s="21"/>
     </row>
     <row r="5" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="63"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
       <c r="K5" s="8"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="64"/>
-      <c r="P5" s="44" t="s">
+      <c r="L5" s="57"/>
+      <c r="M5" s="58"/>
+      <c r="P5" s="39" t="s">
         <v>81</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="62"/>
-      <c r="W5" s="54"/>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="100"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
       <c r="Z5" s="15"/>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="33"/>
+      <c r="AA5" s="101"/>
+      <c r="AB5" s="102"/>
       <c r="AC5" s="10"/>
       <c r="AD5" s="16"/>
       <c r="AE5" s="16"/>
@@ -2074,36 +2076,36 @@
       <c r="EB5" s="16"/>
     </row>
     <row r="6" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="65"/>
-      <c r="P6" s="44" t="s">
+      <c r="L6" s="49"/>
+      <c r="M6" s="59"/>
+      <c r="P6" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="Q6" s="54"/>
+      <c r="Q6" s="49"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="62"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="54"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="100"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
       <c r="Z6" s="15"/>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="33"/>
+      <c r="AA6" s="101"/>
+      <c r="AB6" s="102"/>
       <c r="AC6" s="10"/>
       <c r="AD6" s="16"/>
       <c r="AE6" s="16"/>
@@ -2210,69 +2212,69 @@
       <c r="EB6" s="16"/>
     </row>
     <row r="7" spans="1:133" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="44" t="s">
+      <c r="O7" s="92"/>
+      <c r="P7" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
       <c r="S7" s="5"/>
-      <c r="T7" s="54"/>
-      <c r="U7" s="65"/>
-      <c r="V7" s="62"/>
-      <c r="W7" s="54"/>
-      <c r="X7" s="54"/>
-      <c r="Y7" s="54"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="59"/>
+      <c r="V7" s="100"/>
+      <c r="W7" s="49"/>
+      <c r="X7" s="49"/>
+      <c r="Y7" s="49"/>
       <c r="Z7" s="15"/>
-      <c r="AA7" s="32"/>
-      <c r="AB7" s="33"/>
+      <c r="AA7" s="101"/>
+      <c r="AB7" s="102"/>
       <c r="AC7" s="10"/>
     </row>
     <row r="8" spans="1:133" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="101"/>
-      <c r="P8" s="44" t="s">
+      <c r="O8" s="93"/>
+      <c r="P8" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
-      <c r="U8" s="65"/>
-      <c r="V8" s="62"/>
-      <c r="W8" s="54"/>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="54"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="59"/>
+      <c r="V8" s="100"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="49"/>
       <c r="Z8" s="15"/>
-      <c r="AA8" s="32"/>
-      <c r="AB8" s="33"/>
+      <c r="AA8" s="101"/>
+      <c r="AB8" s="102"/>
       <c r="AC8" s="10"/>
       <c r="AD8" s="25"/>
       <c r="AE8" s="25"/>
@@ -2380,36 +2382,36 @@
       <c r="EC8" s="25"/>
     </row>
     <row r="9" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="100"/>
-      <c r="P9" s="44" t="s">
+      <c r="O9" s="92"/>
+      <c r="P9" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="54"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="54"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="62"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="100"/>
       <c r="W9" s="5"/>
-      <c r="X9" s="54"/>
-      <c r="Y9" s="54"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="49"/>
       <c r="Z9" s="15"/>
-      <c r="AA9" s="32"/>
-      <c r="AB9" s="33"/>
+      <c r="AA9" s="101"/>
+      <c r="AB9" s="102"/>
       <c r="AC9" s="10"/>
       <c r="AD9" s="18"/>
       <c r="AE9" s="18"/>
@@ -2517,7 +2519,7 @@
       <c r="EC9" s="18"/>
     </row>
     <row r="10" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -2531,20 +2533,20 @@
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
       <c r="N10" s="16"/>
-      <c r="O10" s="100"/>
-      <c r="P10" s="37"/>
+      <c r="O10" s="92"/>
+      <c r="P10" s="34"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
       <c r="T10" s="16"/>
       <c r="U10" s="16"/>
-      <c r="V10" s="62"/>
+      <c r="V10" s="100"/>
       <c r="W10" s="16"/>
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
       <c r="Z10" s="16"/>
-      <c r="AA10" s="32"/>
-      <c r="AB10" s="33"/>
+      <c r="AA10" s="101"/>
+      <c r="AB10" s="102"/>
       <c r="AC10" s="10"/>
       <c r="AD10" s="18"/>
       <c r="AE10" s="18"/>
@@ -2652,38 +2654,38 @@
       <c r="EC10" s="18"/>
     </row>
     <row r="11" spans="1:133" s="4" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
       <c r="K11" s="24"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="100"/>
-      <c r="P11" s="70" t="s">
+      <c r="O11" s="92"/>
+      <c r="P11" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="47"/>
-      <c r="S11" s="47"/>
-      <c r="T11" s="47"/>
-      <c r="U11" s="47"/>
-      <c r="V11" s="62"/>
-      <c r="W11" s="47"/>
-      <c r="X11" s="47"/>
-      <c r="Y11" s="47"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="V11" s="100"/>
+      <c r="W11" s="42"/>
+      <c r="X11" s="42"/>
+      <c r="Y11" s="42"/>
       <c r="Z11" s="15"/>
-      <c r="AA11" s="32"/>
-      <c r="AB11" s="33"/>
+      <c r="AA11" s="101"/>
+      <c r="AB11" s="102"/>
       <c r="AC11" s="10"/>
       <c r="AD11" s="18"/>
       <c r="AE11" s="18"/>
@@ -2791,73 +2793,73 @@
       <c r="EC11" s="18"/>
     </row>
     <row r="12" spans="1:133" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="100"/>
-      <c r="P12" s="44" t="s">
+      <c r="O12" s="92"/>
+      <c r="P12" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="54"/>
-      <c r="S12" s="54"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
-      <c r="V12" s="62"/>
-      <c r="W12" s="54"/>
-      <c r="X12" s="54"/>
-      <c r="Y12" s="54"/>
+      <c r="V12" s="100"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="49"/>
       <c r="Z12" s="15"/>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="33"/>
+      <c r="AA12" s="101"/>
+      <c r="AB12" s="102"/>
       <c r="AC12" s="10"/>
     </row>
     <row r="13" spans="1:133" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="101"/>
-      <c r="P13" s="44" t="s">
+      <c r="O13" s="93"/>
+      <c r="P13" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="54"/>
-      <c r="S13" s="54"/>
-      <c r="T13" s="54"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
       <c r="U13" s="5"/>
-      <c r="V13" s="62"/>
-      <c r="W13" s="54"/>
-      <c r="X13" s="54"/>
-      <c r="Y13" s="54"/>
+      <c r="V13" s="100"/>
+      <c r="W13" s="49"/>
+      <c r="X13" s="49"/>
+      <c r="Y13" s="49"/>
       <c r="Z13" s="15"/>
-      <c r="AA13" s="32"/>
-      <c r="AB13" s="33"/>
+      <c r="AA13" s="101"/>
+      <c r="AB13" s="102"/>
       <c r="AC13" s="10"/>
       <c r="AD13" s="16"/>
       <c r="AE13" s="16"/>
@@ -2866,38 +2868,38 @@
       <c r="AH13" s="16"/>
     </row>
     <row r="14" spans="1:133" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="100"/>
-      <c r="P14" s="44" t="s">
+      <c r="O14" s="92"/>
+      <c r="P14" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
       <c r="U14" s="5"/>
-      <c r="V14" s="62"/>
-      <c r="W14" s="54"/>
-      <c r="X14" s="54"/>
-      <c r="Y14" s="54"/>
+      <c r="V14" s="100"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="49"/>
       <c r="Z14" s="15"/>
-      <c r="AA14" s="32"/>
-      <c r="AB14" s="33"/>
+      <c r="AA14" s="101"/>
+      <c r="AB14" s="102"/>
       <c r="AC14" s="10"/>
       <c r="AD14" s="16"/>
       <c r="AE14" s="16"/>
@@ -2906,34 +2908,34 @@
       <c r="AH14" s="16"/>
     </row>
     <row r="15" spans="1:133" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
-      <c r="F15" s="93"/>
+      <c r="F15" s="87"/>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
-      <c r="K15" s="80"/>
+      <c r="K15" s="74"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
-      <c r="O15" s="100"/>
-      <c r="P15" s="80"/>
+      <c r="O15" s="92"/>
+      <c r="P15" s="74"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="18"/>
       <c r="S15" s="18"/>
       <c r="T15" s="18"/>
       <c r="U15" s="18"/>
-      <c r="V15" s="62"/>
+      <c r="V15" s="100"/>
       <c r="W15" s="16"/>
       <c r="X15" s="16"/>
       <c r="Y15" s="16"/>
       <c r="Z15" s="16"/>
-      <c r="AA15" s="32"/>
-      <c r="AB15" s="33"/>
+      <c r="AA15" s="101"/>
+      <c r="AB15" s="102"/>
       <c r="AC15" s="10"/>
       <c r="AD15" s="16"/>
       <c r="AE15" s="16"/>
@@ -2942,38 +2944,38 @@
       <c r="AH15" s="16"/>
     </row>
     <row r="16" spans="1:133" s="27" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
       <c r="K16" s="19"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="53"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="100"/>
-      <c r="P16" s="90" t="s">
+      <c r="O16" s="92"/>
+      <c r="P16" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="47"/>
-      <c r="S16" s="47"/>
-      <c r="T16" s="47"/>
-      <c r="U16" s="47"/>
-      <c r="V16" s="62"/>
-      <c r="W16" s="47"/>
-      <c r="X16" s="47"/>
-      <c r="Y16" s="47"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42"/>
+      <c r="V16" s="100"/>
+      <c r="W16" s="42"/>
+      <c r="X16" s="42"/>
+      <c r="Y16" s="42"/>
       <c r="Z16" s="15"/>
-      <c r="AA16" s="32"/>
-      <c r="AB16" s="33"/>
+      <c r="AA16" s="101"/>
+      <c r="AB16" s="102"/>
       <c r="AC16" s="10"/>
       <c r="AD16" s="16"/>
       <c r="AE16" s="16"/>
@@ -2982,73 +2984,73 @@
       <c r="AH16" s="16"/>
     </row>
     <row r="17" spans="1:133" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="100"/>
-      <c r="P17" s="44" t="s">
+      <c r="O17" s="92"/>
+      <c r="P17" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
-      <c r="V17" s="62"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="54"/>
+      <c r="V17" s="100"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="49"/>
       <c r="Z17" s="15"/>
-      <c r="AA17" s="32"/>
-      <c r="AB17" s="33"/>
+      <c r="AA17" s="101"/>
+      <c r="AB17" s="102"/>
       <c r="AC17" s="10"/>
     </row>
     <row r="18" spans="1:133" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="101"/>
-      <c r="P18" s="44" t="s">
+      <c r="O18" s="93"/>
+      <c r="P18" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="62"/>
-      <c r="W18" s="54"/>
-      <c r="X18" s="54"/>
-      <c r="Y18" s="54"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="49"/>
+      <c r="V18" s="100"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="49"/>
+      <c r="Y18" s="49"/>
       <c r="Z18" s="15"/>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="33"/>
+      <c r="AA18" s="101"/>
+      <c r="AB18" s="102"/>
       <c r="AC18" s="10"/>
       <c r="AD18" s="25"/>
       <c r="AE18" s="25"/>
@@ -3156,40 +3158,40 @@
       <c r="EC18" s="25"/>
     </row>
     <row r="19" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
       <c r="K19" s="6"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
       <c r="N19" s="10"/>
-      <c r="O19" s="100"/>
-      <c r="P19" s="44" t="s">
+      <c r="O19" s="92"/>
+      <c r="P19" s="39" t="s">
         <v>88</v>
       </c>
       <c r="Q19" s="5"/>
-      <c r="R19" s="54"/>
-      <c r="S19" s="54"/>
-      <c r="T19" s="54"/>
-      <c r="U19" s="54"/>
-      <c r="V19" s="62"/>
-      <c r="W19" s="54" t="s">
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="49"/>
+      <c r="V19" s="100"/>
+      <c r="W19" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="X19" s="54"/>
-      <c r="Y19" s="54"/>
+      <c r="X19" s="49"/>
+      <c r="Y19" s="49"/>
       <c r="Z19" s="15"/>
-      <c r="AA19" s="32"/>
-      <c r="AB19" s="33"/>
+      <c r="AA19" s="101"/>
+      <c r="AB19" s="102"/>
       <c r="AC19" s="10"/>
       <c r="AD19" s="18"/>
       <c r="AE19" s="18"/>
@@ -3297,38 +3299,38 @@
       <c r="EC19" s="18"/>
     </row>
     <row r="20" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="53"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
       <c r="K20" s="24"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="100"/>
-      <c r="P20" s="44" t="s">
+      <c r="O20" s="92"/>
+      <c r="P20" s="39" t="s">
         <v>92</v>
       </c>
       <c r="Q20" s="5"/>
-      <c r="R20" s="54"/>
-      <c r="S20" s="54"/>
-      <c r="T20" s="54"/>
-      <c r="U20" s="54"/>
-      <c r="V20" s="62"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="49"/>
+      <c r="V20" s="100"/>
       <c r="W20" s="5"/>
-      <c r="X20" s="54"/>
-      <c r="Y20" s="54"/>
+      <c r="X20" s="49"/>
+      <c r="Y20" s="49"/>
       <c r="Z20" s="15"/>
-      <c r="AA20" s="32"/>
-      <c r="AB20" s="33"/>
+      <c r="AA20" s="101"/>
+      <c r="AB20" s="102"/>
       <c r="AC20" s="10"/>
       <c r="AD20" s="18"/>
       <c r="AE20" s="18"/>
@@ -3436,38 +3438,38 @@
       <c r="EC20" s="18"/>
     </row>
     <row r="21" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="54"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
       <c r="N21" s="10"/>
-      <c r="O21" s="100"/>
-      <c r="P21" s="44" t="s">
+      <c r="O21" s="92"/>
+      <c r="P21" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="Q21" s="54"/>
+      <c r="Q21" s="49"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
-      <c r="T21" s="54"/>
-      <c r="U21" s="54"/>
-      <c r="V21" s="62"/>
-      <c r="W21" s="54"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="49"/>
+      <c r="V21" s="100"/>
+      <c r="W21" s="49"/>
       <c r="X21" s="5"/>
-      <c r="Y21" s="54"/>
+      <c r="Y21" s="49"/>
       <c r="Z21" s="15"/>
-      <c r="AA21" s="32"/>
-      <c r="AB21" s="33"/>
+      <c r="AA21" s="101"/>
+      <c r="AB21" s="102"/>
       <c r="AC21" s="10"/>
       <c r="AD21" s="18"/>
       <c r="AE21" s="18"/>
@@ -3575,24 +3577,24 @@
       <c r="EC21" s="18"/>
     </row>
     <row r="22" spans="1:133" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
       <c r="K22" s="6"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="100"/>
-      <c r="P22" s="44" t="s">
+      <c r="O22" s="92"/>
+      <c r="P22" s="39" t="s">
         <v>91</v>
       </c>
       <c r="Q22" s="5"/>
@@ -3600,48 +3602,48 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
-      <c r="V22" s="62"/>
+      <c r="V22" s="100"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="15"/>
-      <c r="AA22" s="32"/>
-      <c r="AB22" s="33"/>
+      <c r="AA22" s="101"/>
+      <c r="AB22" s="102"/>
       <c r="AC22" s="10"/>
     </row>
     <row r="23" spans="1:133" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
       <c r="N23" s="10"/>
-      <c r="O23" s="101"/>
-      <c r="P23" s="44" t="s">
+      <c r="O23" s="93"/>
+      <c r="P23" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="54"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="62"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="49"/>
+      <c r="U23" s="49"/>
+      <c r="V23" s="100"/>
       <c r="W23" s="5"/>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="54"/>
+      <c r="X23" s="49"/>
+      <c r="Y23" s="49"/>
       <c r="Z23" s="15"/>
-      <c r="AA23" s="32"/>
-      <c r="AB23" s="33"/>
+      <c r="AA23" s="101"/>
+      <c r="AB23" s="102"/>
       <c r="AC23" s="10"/>
       <c r="AD23" s="25"/>
       <c r="AE23" s="25"/>
@@ -3749,7 +3751,7 @@
       <c r="EC23" s="25"/>
     </row>
     <row r="24" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="72"/>
+      <c r="A24" s="66"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
@@ -3763,22 +3765,22 @@
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
-      <c r="O24" s="100"/>
-      <c r="P24" s="44" t="s">
+      <c r="O24" s="92"/>
+      <c r="P24" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="54"/>
-      <c r="S24" s="54"/>
-      <c r="T24" s="54"/>
-      <c r="U24" s="54"/>
-      <c r="V24" s="62"/>
-      <c r="W24" s="54"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+      <c r="U24" s="49"/>
+      <c r="V24" s="100"/>
+      <c r="W24" s="49"/>
       <c r="X24" s="5"/>
-      <c r="Y24" s="54"/>
+      <c r="Y24" s="49"/>
       <c r="Z24" s="15"/>
-      <c r="AA24" s="32"/>
-      <c r="AB24" s="33"/>
+      <c r="AA24" s="101"/>
+      <c r="AB24" s="102"/>
       <c r="AC24" s="10"/>
       <c r="AD24" s="18"/>
       <c r="AE24" s="18"/>
@@ -3886,38 +3888,38 @@
       <c r="EC24" s="18"/>
     </row>
     <row r="25" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
       <c r="N25" s="10"/>
-      <c r="O25" s="100"/>
-      <c r="P25" s="44" t="s">
+      <c r="O25" s="92"/>
+      <c r="P25" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="54"/>
-      <c r="T25" s="54"/>
-      <c r="U25" s="54"/>
-      <c r="V25" s="62"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="49"/>
+      <c r="U25" s="49"/>
+      <c r="V25" s="100"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
-      <c r="Y25" s="54"/>
+      <c r="Y25" s="49"/>
       <c r="Z25" s="15"/>
-      <c r="AA25" s="32"/>
-      <c r="AB25" s="33"/>
+      <c r="AA25" s="101"/>
+      <c r="AB25" s="102"/>
       <c r="AC25" s="10"/>
       <c r="AD25" s="18"/>
       <c r="AE25" s="18"/>
@@ -4025,38 +4027,38 @@
       <c r="EC25" s="18"/>
     </row>
     <row r="26" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
       <c r="K26" s="6"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="10"/>
-      <c r="O26" s="100"/>
-      <c r="P26" s="44" t="s">
+      <c r="O26" s="92"/>
+      <c r="P26" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="54"/>
-      <c r="S26" s="54"/>
-      <c r="T26" s="54"/>
-      <c r="U26" s="54"/>
-      <c r="V26" s="62"/>
-      <c r="W26" s="54"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="49"/>
+      <c r="U26" s="49"/>
+      <c r="V26" s="100"/>
+      <c r="W26" s="49"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
       <c r="Z26" s="15"/>
-      <c r="AA26" s="32"/>
-      <c r="AB26" s="33"/>
+      <c r="AA26" s="101"/>
+      <c r="AB26" s="102"/>
       <c r="AC26" s="10"/>
       <c r="AD26" s="18"/>
       <c r="AE26" s="18"/>
@@ -4164,73 +4166,73 @@
       <c r="EC26" s="18"/>
     </row>
     <row r="27" spans="1:133" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
       <c r="K27" s="6"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="10"/>
-      <c r="O27" s="100"/>
-      <c r="P27" s="44" t="s">
+      <c r="O27" s="92"/>
+      <c r="P27" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="Q27" s="54"/>
-      <c r="R27" s="54"/>
-      <c r="S27" s="54"/>
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
       <c r="T27" s="5"/>
-      <c r="U27" s="54"/>
-      <c r="V27" s="62"/>
-      <c r="W27" s="54"/>
-      <c r="X27" s="54"/>
-      <c r="Y27" s="54"/>
+      <c r="U27" s="49"/>
+      <c r="V27" s="100"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="49"/>
+      <c r="Y27" s="49"/>
       <c r="Z27" s="15"/>
-      <c r="AA27" s="32"/>
-      <c r="AB27" s="33"/>
+      <c r="AA27" s="101"/>
+      <c r="AB27" s="102"/>
       <c r="AC27" s="10"/>
     </row>
     <row r="28" spans="1:133" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="54"/>
+      <c r="J28" s="49"/>
       <c r="K28" s="6"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="101"/>
-      <c r="P28" s="44" t="s">
+      <c r="O28" s="93"/>
+      <c r="P28" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="Q28" s="54"/>
-      <c r="R28" s="54"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
       <c r="S28" s="5"/>
-      <c r="T28" s="54"/>
-      <c r="U28" s="54"/>
-      <c r="V28" s="62"/>
-      <c r="W28" s="54"/>
-      <c r="X28" s="54"/>
-      <c r="Y28" s="54"/>
+      <c r="T28" s="49"/>
+      <c r="U28" s="49"/>
+      <c r="V28" s="100"/>
+      <c r="W28" s="49"/>
+      <c r="X28" s="49"/>
+      <c r="Y28" s="49"/>
       <c r="Z28" s="15"/>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="33"/>
+      <c r="AA28" s="101"/>
+      <c r="AB28" s="102"/>
       <c r="AC28" s="10"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25"/>
@@ -4338,34 +4340,34 @@
       <c r="EC28" s="25"/>
     </row>
     <row r="29" spans="1:133" s="4" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
       <c r="N29" s="10"/>
-      <c r="O29" s="100"/>
-      <c r="P29" s="44"/>
-      <c r="Q29" s="54"/>
-      <c r="R29" s="54"/>
-      <c r="S29" s="54"/>
-      <c r="T29" s="54"/>
-      <c r="U29" s="54"/>
-      <c r="V29" s="62"/>
-      <c r="W29" s="54"/>
-      <c r="X29" s="54"/>
-      <c r="Y29" s="54"/>
+      <c r="O29" s="92"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="49"/>
+      <c r="U29" s="49"/>
+      <c r="V29" s="100"/>
+      <c r="W29" s="49"/>
+      <c r="X29" s="49"/>
+      <c r="Y29" s="49"/>
       <c r="Z29" s="15"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="33"/>
+      <c r="AA29" s="101"/>
+      <c r="AB29" s="102"/>
       <c r="AC29" s="10"/>
       <c r="AD29" s="18"/>
       <c r="AE29" s="18"/>
@@ -4473,13 +4475,13 @@
       <c r="EC29" s="18"/>
     </row>
     <row r="30" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
-      <c r="G30" s="93"/>
+      <c r="G30" s="87"/>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
@@ -4487,20 +4489,20 @@
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
-      <c r="O30" s="100"/>
-      <c r="P30" s="81"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="51"/>
-      <c r="T30" s="51"/>
-      <c r="U30" s="51"/>
-      <c r="V30" s="62"/>
+      <c r="O30" s="92"/>
+      <c r="P30" s="75"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="46"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="46"/>
+      <c r="V30" s="100"/>
       <c r="W30" s="16"/>
       <c r="X30" s="16"/>
       <c r="Y30" s="16"/>
       <c r="Z30" s="15"/>
-      <c r="AA30" s="32"/>
-      <c r="AB30" s="33"/>
+      <c r="AA30" s="101"/>
+      <c r="AB30" s="102"/>
       <c r="AC30" s="10"/>
       <c r="AD30" s="18"/>
       <c r="AE30" s="18"/>
@@ -4608,38 +4610,38 @@
       <c r="EC30" s="18"/>
     </row>
     <row r="31" spans="1:133" s="4" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="90" t="s">
+      <c r="A31" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="92"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
       <c r="K31" s="19"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="52"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
       <c r="N31" s="10"/>
-      <c r="O31" s="100"/>
-      <c r="P31" s="91" t="s">
+      <c r="O31" s="92"/>
+      <c r="P31" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="52"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="62"/>
-      <c r="W31" s="47"/>
-      <c r="X31" s="47"/>
-      <c r="Y31" s="47"/>
+      <c r="Q31" s="47"/>
+      <c r="R31" s="47"/>
+      <c r="S31" s="47"/>
+      <c r="T31" s="47"/>
+      <c r="U31" s="47"/>
+      <c r="V31" s="100"/>
+      <c r="W31" s="42"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
       <c r="Z31" s="15"/>
-      <c r="AA31" s="32"/>
-      <c r="AB31" s="33"/>
+      <c r="AA31" s="101"/>
+      <c r="AB31" s="102"/>
       <c r="AC31" s="10"/>
       <c r="AD31" s="18"/>
       <c r="AE31" s="18"/>
@@ -4747,38 +4749,38 @@
       <c r="EC31" s="18"/>
     </row>
     <row r="32" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="6"/>
-      <c r="L32" s="54"/>
-      <c r="M32" s="54"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
       <c r="N32" s="10"/>
-      <c r="O32" s="100"/>
-      <c r="P32" s="82" t="s">
+      <c r="O32" s="92"/>
+      <c r="P32" s="76" t="s">
         <v>97</v>
       </c>
       <c r="Q32" s="5"/>
-      <c r="R32" s="54"/>
-      <c r="S32" s="54"/>
-      <c r="T32" s="54"/>
-      <c r="U32" s="54"/>
-      <c r="V32" s="62"/>
-      <c r="W32" s="54"/>
-      <c r="X32" s="54"/>
-      <c r="Y32" s="54"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="49"/>
+      <c r="U32" s="49"/>
+      <c r="V32" s="100"/>
+      <c r="W32" s="49"/>
+      <c r="X32" s="49"/>
+      <c r="Y32" s="49"/>
       <c r="Z32" s="15"/>
-      <c r="AA32" s="32"/>
-      <c r="AB32" s="33"/>
+      <c r="AA32" s="101"/>
+      <c r="AB32" s="102"/>
       <c r="AC32" s="10"/>
       <c r="AD32" s="18"/>
       <c r="AE32" s="18"/>
@@ -4886,73 +4888,73 @@
       <c r="EC32" s="18"/>
     </row>
     <row r="33" spans="1:133" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="6"/>
-      <c r="L33" s="54"/>
-      <c r="M33" s="54"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
       <c r="N33" s="10"/>
-      <c r="O33" s="100"/>
-      <c r="P33" s="82" t="s">
+      <c r="O33" s="92"/>
+      <c r="P33" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="Q33" s="54"/>
+      <c r="Q33" s="49"/>
       <c r="R33" s="5"/>
-      <c r="S33" s="54"/>
-      <c r="T33" s="54"/>
-      <c r="U33" s="54"/>
-      <c r="V33" s="62"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="49"/>
+      <c r="V33" s="100"/>
       <c r="W33" s="5"/>
-      <c r="X33" s="54"/>
-      <c r="Y33" s="54"/>
+      <c r="X33" s="49"/>
+      <c r="Y33" s="49"/>
       <c r="Z33" s="15"/>
-      <c r="AA33" s="32"/>
-      <c r="AB33" s="33"/>
+      <c r="AA33" s="101"/>
+      <c r="AB33" s="102"/>
       <c r="AC33" s="10"/>
     </row>
     <row r="34" spans="1:133" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="6"/>
-      <c r="L34" s="54"/>
-      <c r="M34" s="54"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
       <c r="N34" s="10"/>
-      <c r="O34" s="102"/>
-      <c r="P34" s="82" t="s">
+      <c r="O34" s="94"/>
+      <c r="P34" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="Q34" s="54"/>
-      <c r="R34" s="54"/>
-      <c r="S34" s="54"/>
-      <c r="T34" s="54"/>
-      <c r="U34" s="54"/>
-      <c r="V34" s="62"/>
-      <c r="W34" s="53"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="49"/>
+      <c r="V34" s="100"/>
+      <c r="W34" s="48"/>
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
       <c r="Z34" s="15"/>
-      <c r="AA34" s="32"/>
-      <c r="AB34" s="33"/>
+      <c r="AA34" s="101"/>
+      <c r="AB34" s="102"/>
       <c r="AC34" s="10"/>
       <c r="AD34" s="25"/>
       <c r="AE34" s="25"/>
@@ -5060,38 +5062,38 @@
       <c r="EC34" s="25"/>
     </row>
     <row r="35" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="6"/>
-      <c r="L35" s="54"/>
-      <c r="M35" s="54"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
       <c r="N35" s="10"/>
-      <c r="O35" s="103"/>
-      <c r="P35" s="82" t="s">
+      <c r="O35" s="95"/>
+      <c r="P35" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="Q35" s="54"/>
-      <c r="R35" s="54"/>
-      <c r="S35" s="54"/>
-      <c r="T35" s="54"/>
-      <c r="U35" s="54"/>
-      <c r="V35" s="62"/>
-      <c r="W35" s="54"/>
-      <c r="X35" s="54"/>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="49"/>
+      <c r="U35" s="49"/>
+      <c r="V35" s="100"/>
+      <c r="W35" s="49"/>
+      <c r="X35" s="49"/>
       <c r="Y35" s="5"/>
       <c r="Z35" s="15"/>
-      <c r="AA35" s="32"/>
-      <c r="AB35" s="33"/>
+      <c r="AA35" s="101"/>
+      <c r="AB35" s="102"/>
       <c r="AC35" s="10"/>
       <c r="AD35" s="18"/>
       <c r="AE35" s="18"/>
@@ -5199,36 +5201,36 @@
       <c r="EC35" s="18"/>
     </row>
     <row r="36" spans="1:133" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="54"/>
+      <c r="A36" s="49"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
       <c r="N36" s="10"/>
-      <c r="O36" s="103"/>
-      <c r="P36" s="82" t="s">
+      <c r="O36" s="95"/>
+      <c r="P36" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="54"/>
-      <c r="S36" s="54"/>
-      <c r="T36" s="54"/>
-      <c r="U36" s="54"/>
-      <c r="V36" s="62"/>
-      <c r="W36" s="54"/>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="49"/>
+      <c r="U36" s="49"/>
+      <c r="V36" s="100"/>
+      <c r="W36" s="49"/>
       <c r="X36" s="5"/>
-      <c r="Y36" s="54"/>
+      <c r="Y36" s="49"/>
       <c r="Z36" s="15"/>
-      <c r="AA36" s="32"/>
-      <c r="AB36" s="33"/>
+      <c r="AA36" s="101"/>
+      <c r="AB36" s="102"/>
       <c r="AC36" s="10"/>
       <c r="AD36" s="18"/>
       <c r="AE36" s="18"/>
@@ -5336,7 +5338,7 @@
       <c r="EC36" s="18"/>
     </row>
     <row r="37" spans="1:133" s="4" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -5350,8 +5352,8 @@
       <c r="L37" s="16"/>
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
-      <c r="O37" s="103"/>
-      <c r="P37" s="37"/>
+      <c r="O37" s="95"/>
+      <c r="P37" s="34"/>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
       <c r="S37" s="16"/>
@@ -5471,76 +5473,76 @@
       <c r="EC37" s="18"/>
     </row>
     <row r="38" spans="1:133" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="71" t="s">
+      <c r="A38" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="106" t="s">
+      <c r="B38" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
+      <c r="C38" s="104"/>
+      <c r="D38" s="104"/>
+      <c r="E38" s="104"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="104"/>
+      <c r="H38" s="104"/>
+      <c r="I38" s="104"/>
+      <c r="J38" s="104"/>
+      <c r="K38" s="104"/>
+      <c r="L38" s="104"/>
+      <c r="M38" s="104"/>
       <c r="N38" s="28"/>
-      <c r="O38" s="100"/>
-      <c r="P38" s="71" t="s">
+      <c r="O38" s="92"/>
+      <c r="P38" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="Q38" s="106" t="s">
+      <c r="Q38" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
+      <c r="R38" s="104"/>
+      <c r="S38" s="104"/>
+      <c r="T38" s="104"/>
+      <c r="U38" s="104"/>
+      <c r="V38" s="104"/>
+      <c r="W38" s="104"/>
+      <c r="X38" s="104"/>
+      <c r="Y38" s="104"/>
+      <c r="Z38" s="104"/>
+      <c r="AA38" s="104"/>
+      <c r="AB38" s="104"/>
       <c r="AC38" s="28"/>
     </row>
     <row r="39" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="107"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="39"/>
+      <c r="B39" s="105"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="106"/>
+      <c r="F39" s="106"/>
+      <c r="G39" s="106"/>
+      <c r="H39" s="106"/>
+      <c r="I39" s="106"/>
+      <c r="J39" s="106"/>
+      <c r="K39" s="106"/>
+      <c r="L39" s="106"/>
+      <c r="M39" s="106"/>
       <c r="N39" s="27"/>
-      <c r="P39" s="38" t="s">
+      <c r="P39" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="Q39" s="107"/>
-      <c r="R39" s="39"/>
-      <c r="S39" s="39"/>
-      <c r="T39" s="39"/>
-      <c r="U39" s="39"/>
-      <c r="V39" s="39"/>
-      <c r="W39" s="39"/>
-      <c r="X39" s="39"/>
-      <c r="Y39" s="39"/>
-      <c r="Z39" s="39"/>
-      <c r="AA39" s="39"/>
-      <c r="AB39" s="39"/>
+      <c r="Q39" s="105"/>
+      <c r="R39" s="106"/>
+      <c r="S39" s="106"/>
+      <c r="T39" s="106"/>
+      <c r="U39" s="106"/>
+      <c r="V39" s="106"/>
+      <c r="W39" s="106"/>
+      <c r="X39" s="106"/>
+      <c r="Y39" s="106"/>
+      <c r="Z39" s="106"/>
+      <c r="AA39" s="106"/>
+      <c r="AB39" s="106"/>
       <c r="AC39" s="27"/>
       <c r="AD39" s="16"/>
       <c r="AE39" s="16"/>
@@ -5647,37 +5649,37 @@
       <c r="EB39" s="16"/>
     </row>
     <row r="40" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="107"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-      <c r="M40" s="39"/>
+      <c r="B40" s="105"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="106"/>
+      <c r="F40" s="106"/>
+      <c r="G40" s="106"/>
+      <c r="H40" s="106"/>
+      <c r="I40" s="106"/>
+      <c r="J40" s="106"/>
+      <c r="K40" s="106"/>
+      <c r="L40" s="106"/>
+      <c r="M40" s="106"/>
       <c r="N40" s="27"/>
-      <c r="P40" s="38" t="s">
+      <c r="P40" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="Q40" s="107"/>
-      <c r="R40" s="39"/>
-      <c r="S40" s="39"/>
-      <c r="T40" s="39"/>
-      <c r="U40" s="39"/>
-      <c r="V40" s="39"/>
-      <c r="W40" s="39"/>
-      <c r="X40" s="39"/>
-      <c r="Y40" s="39"/>
-      <c r="Z40" s="39"/>
-      <c r="AA40" s="39"/>
-      <c r="AB40" s="39"/>
+      <c r="Q40" s="105"/>
+      <c r="R40" s="106"/>
+      <c r="S40" s="106"/>
+      <c r="T40" s="106"/>
+      <c r="U40" s="106"/>
+      <c r="V40" s="106"/>
+      <c r="W40" s="106"/>
+      <c r="X40" s="106"/>
+      <c r="Y40" s="106"/>
+      <c r="Z40" s="106"/>
+      <c r="AA40" s="106"/>
+      <c r="AB40" s="106"/>
       <c r="AC40" s="27"/>
       <c r="AD40" s="16"/>
       <c r="AE40" s="16"/>
@@ -5784,37 +5786,37 @@
       <c r="EB40" s="16"/>
     </row>
     <row r="41" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="108"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="40"/>
+      <c r="B41" s="107"/>
+      <c r="C41" s="108"/>
+      <c r="D41" s="108"/>
+      <c r="E41" s="108"/>
+      <c r="F41" s="108"/>
+      <c r="G41" s="108"/>
+      <c r="H41" s="108"/>
+      <c r="I41" s="108"/>
+      <c r="J41" s="108"/>
+      <c r="K41" s="108"/>
+      <c r="L41" s="108"/>
+      <c r="M41" s="108"/>
       <c r="N41" s="27"/>
-      <c r="P41" s="38" t="s">
+      <c r="P41" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="Q41" s="108"/>
-      <c r="R41" s="40"/>
-      <c r="S41" s="40"/>
-      <c r="T41" s="40"/>
-      <c r="U41" s="40"/>
-      <c r="V41" s="40"/>
-      <c r="W41" s="40"/>
-      <c r="X41" s="40"/>
-      <c r="Y41" s="40"/>
-      <c r="Z41" s="40"/>
-      <c r="AA41" s="40"/>
-      <c r="AB41" s="40"/>
+      <c r="Q41" s="107"/>
+      <c r="R41" s="108"/>
+      <c r="S41" s="108"/>
+      <c r="T41" s="108"/>
+      <c r="U41" s="108"/>
+      <c r="V41" s="108"/>
+      <c r="W41" s="108"/>
+      <c r="X41" s="108"/>
+      <c r="Y41" s="108"/>
+      <c r="Z41" s="108"/>
+      <c r="AA41" s="108"/>
+      <c r="AB41" s="108"/>
       <c r="AC41" s="27"/>
       <c r="AD41" s="16"/>
       <c r="AE41" s="16"/>
@@ -5921,7 +5923,7 @@
       <c r="EB41" s="16"/>
     </row>
     <row r="42" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
+      <c r="A42" s="34"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -5935,7 +5937,7 @@
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
       <c r="N42" s="16"/>
-      <c r="P42" s="37"/>
+      <c r="P42" s="34"/>
       <c r="Q42" s="16"/>
       <c r="R42" s="16"/>
       <c r="S42" s="16"/>
@@ -6054,7 +6056,7 @@
       <c r="EB42" s="16"/>
     </row>
     <row r="43" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A43" s="37"/>
+      <c r="A43" s="34"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -6068,7 +6070,7 @@
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
-      <c r="P43" s="37"/>
+      <c r="P43" s="34"/>
       <c r="Q43" s="16"/>
       <c r="R43" s="16"/>
       <c r="S43" s="16"/>
@@ -6187,12 +6189,12 @@
       <c r="EB43" s="16"/>
     </row>
     <row r="44" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="61"/>
-      <c r="O44" s="104"/>
-      <c r="P44" s="37"/>
+      <c r="G44" s="56"/>
+      <c r="O44" s="96"/>
+      <c r="P44" s="34"/>
       <c r="Q44" s="16"/>
       <c r="R44" s="16"/>
       <c r="S44" s="16"/>
@@ -6311,14 +6313,14 @@
       <c r="EB44" s="16"/>
     </row>
     <row r="45" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G45" s="61"/>
-      <c r="O45" s="104"/>
-      <c r="P45" s="97"/>
-      <c r="Q45" s="96"/>
-      <c r="R45" s="96"/>
+      <c r="G45" s="56"/>
+      <c r="O45" s="96"/>
+      <c r="P45" s="89"/>
+      <c r="Q45" s="88"/>
+      <c r="R45" s="88"/>
       <c r="S45" s="16"/>
       <c r="T45" s="16"/>
       <c r="U45" s="16"/>
@@ -6435,14 +6437,14 @@
       <c r="EB45" s="16"/>
     </row>
     <row r="46" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="G46" s="61"/>
-      <c r="O46" s="104"/>
-      <c r="P46" s="97"/>
-      <c r="Q46" s="96"/>
-      <c r="R46" s="96"/>
+      <c r="G46" s="56"/>
+      <c r="O46" s="96"/>
+      <c r="P46" s="89"/>
+      <c r="Q46" s="88"/>
+      <c r="R46" s="88"/>
       <c r="S46" s="16"/>
       <c r="T46" s="16"/>
       <c r="U46" s="16"/>
@@ -6559,14 +6561,14 @@
       <c r="EB46" s="16"/>
     </row>
     <row r="47" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="G47" s="61"/>
-      <c r="O47" s="104"/>
-      <c r="P47" s="97"/>
-      <c r="Q47" s="96"/>
-      <c r="R47" s="96"/>
+      <c r="G47" s="56"/>
+      <c r="O47" s="96"/>
+      <c r="P47" s="89"/>
+      <c r="Q47" s="88"/>
+      <c r="R47" s="88"/>
       <c r="S47" s="16"/>
       <c r="T47" s="16"/>
       <c r="U47" s="16"/>
@@ -6683,14 +6685,14 @@
       <c r="EB47" s="16"/>
     </row>
     <row r="48" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A48" s="45" t="s">
+      <c r="A48" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="G48" s="61"/>
-      <c r="O48" s="104"/>
-      <c r="P48" s="97"/>
-      <c r="Q48" s="96"/>
-      <c r="R48" s="96"/>
+      <c r="G48" s="56"/>
+      <c r="O48" s="96"/>
+      <c r="P48" s="89"/>
+      <c r="Q48" s="88"/>
+      <c r="R48" s="88"/>
       <c r="S48" s="16"/>
       <c r="T48" s="16"/>
       <c r="U48" s="16"/>
@@ -6807,11 +6809,11 @@
       <c r="EB48" s="16"/>
     </row>
     <row r="49" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G49" s="61"/>
-      <c r="O49" s="104"/>
-      <c r="P49" s="97"/>
-      <c r="Q49" s="96"/>
-      <c r="R49" s="96"/>
+      <c r="G49" s="56"/>
+      <c r="O49" s="96"/>
+      <c r="P49" s="89"/>
+      <c r="Q49" s="88"/>
+      <c r="R49" s="88"/>
       <c r="S49" s="16"/>
       <c r="T49" s="16"/>
       <c r="U49" s="16"/>
@@ -6928,14 +6930,14 @@
       <c r="EB49" s="16"/>
     </row>
     <row r="50" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="G50" s="61"/>
-      <c r="O50" s="104"/>
-      <c r="P50" s="97"/>
-      <c r="Q50" s="96"/>
-      <c r="R50" s="96"/>
+      <c r="G50" s="56"/>
+      <c r="O50" s="96"/>
+      <c r="P50" s="89"/>
+      <c r="Q50" s="88"/>
+      <c r="R50" s="88"/>
       <c r="S50" s="16"/>
       <c r="T50" s="16"/>
       <c r="U50" s="16"/>
@@ -7052,14 +7054,14 @@
       <c r="EB50" s="16"/>
     </row>
     <row r="51" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="61"/>
-      <c r="O51" s="104"/>
-      <c r="P51" s="97"/>
-      <c r="Q51" s="96"/>
-      <c r="R51" s="96"/>
+      <c r="G51" s="56"/>
+      <c r="O51" s="96"/>
+      <c r="P51" s="89"/>
+      <c r="Q51" s="88"/>
+      <c r="R51" s="88"/>
       <c r="S51" s="16"/>
       <c r="T51" s="16"/>
       <c r="U51" s="16"/>
@@ -7176,14 +7178,14 @@
       <c r="EB51" s="16"/>
     </row>
     <row r="52" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A52" s="45" t="s">
+      <c r="A52" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="G52" s="61"/>
-      <c r="O52" s="104"/>
-      <c r="P52" s="97"/>
-      <c r="Q52" s="96"/>
-      <c r="R52" s="96"/>
+      <c r="G52" s="56"/>
+      <c r="O52" s="96"/>
+      <c r="P52" s="89"/>
+      <c r="Q52" s="88"/>
+      <c r="R52" s="88"/>
       <c r="S52" s="16"/>
       <c r="T52" s="16"/>
       <c r="U52" s="16"/>
@@ -7300,11 +7302,11 @@
       <c r="EB52" s="16"/>
     </row>
     <row r="53" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G53" s="61"/>
-      <c r="O53" s="104"/>
-      <c r="P53" s="97"/>
-      <c r="Q53" s="96"/>
-      <c r="R53" s="96"/>
+      <c r="G53" s="56"/>
+      <c r="O53" s="96"/>
+      <c r="P53" s="89"/>
+      <c r="Q53" s="88"/>
+      <c r="R53" s="88"/>
       <c r="S53" s="16"/>
       <c r="T53" s="16"/>
       <c r="U53" s="16"/>
@@ -7421,14 +7423,14 @@
       <c r="EB53" s="16"/>
     </row>
     <row r="54" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A54" s="75" t="s">
+      <c r="A54" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G54" s="61"/>
-      <c r="O54" s="104"/>
-      <c r="P54" s="97"/>
-      <c r="Q54" s="96"/>
-      <c r="R54" s="96"/>
+      <c r="G54" s="56"/>
+      <c r="O54" s="96"/>
+      <c r="P54" s="89"/>
+      <c r="Q54" s="88"/>
+      <c r="R54" s="88"/>
       <c r="S54" s="16"/>
       <c r="T54" s="16"/>
       <c r="U54" s="16"/>
@@ -7545,14 +7547,14 @@
       <c r="EB54" s="16"/>
     </row>
     <row r="55" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G55" s="61"/>
-      <c r="O55" s="104"/>
-      <c r="P55" s="97"/>
-      <c r="Q55" s="96"/>
-      <c r="R55" s="96"/>
+      <c r="G55" s="56"/>
+      <c r="O55" s="96"/>
+      <c r="P55" s="89"/>
+      <c r="Q55" s="88"/>
+      <c r="R55" s="88"/>
       <c r="S55" s="16"/>
       <c r="T55" s="16"/>
       <c r="U55" s="16"/>
@@ -7669,14 +7671,14 @@
       <c r="EB55" s="16"/>
     </row>
     <row r="56" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="G56" s="61"/>
-      <c r="O56" s="104"/>
-      <c r="P56" s="97"/>
-      <c r="Q56" s="96"/>
-      <c r="R56" s="96"/>
+      <c r="G56" s="56"/>
+      <c r="O56" s="96"/>
+      <c r="P56" s="89"/>
+      <c r="Q56" s="88"/>
+      <c r="R56" s="88"/>
       <c r="S56" s="16"/>
       <c r="T56" s="16"/>
       <c r="U56" s="16"/>
@@ -7793,14 +7795,14 @@
       <c r="EB56" s="16"/>
     </row>
     <row r="57" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A57" s="45" t="s">
+      <c r="A57" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="G57" s="61"/>
-      <c r="O57" s="104"/>
-      <c r="P57" s="97"/>
-      <c r="Q57" s="96"/>
-      <c r="R57" s="96"/>
+      <c r="G57" s="56"/>
+      <c r="O57" s="96"/>
+      <c r="P57" s="89"/>
+      <c r="Q57" s="88"/>
+      <c r="R57" s="88"/>
       <c r="S57" s="16"/>
       <c r="T57" s="16"/>
       <c r="U57" s="16"/>
@@ -7917,11 +7919,11 @@
       <c r="EB57" s="16"/>
     </row>
     <row r="58" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G58" s="61"/>
-      <c r="O58" s="104"/>
-      <c r="P58" s="97"/>
-      <c r="Q58" s="96"/>
-      <c r="R58" s="96"/>
+      <c r="G58" s="56"/>
+      <c r="O58" s="96"/>
+      <c r="P58" s="89"/>
+      <c r="Q58" s="88"/>
+      <c r="R58" s="88"/>
       <c r="S58" s="16"/>
       <c r="T58" s="16"/>
       <c r="U58" s="16"/>
@@ -8038,14 +8040,14 @@
       <c r="EB58" s="16"/>
     </row>
     <row r="59" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A59" s="75" t="s">
+      <c r="A59" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="G59" s="61"/>
-      <c r="O59" s="104"/>
-      <c r="P59" s="97"/>
-      <c r="Q59" s="96"/>
-      <c r="R59" s="96"/>
+      <c r="G59" s="56"/>
+      <c r="O59" s="96"/>
+      <c r="P59" s="89"/>
+      <c r="Q59" s="88"/>
+      <c r="R59" s="88"/>
       <c r="S59" s="16"/>
       <c r="T59" s="16"/>
       <c r="U59" s="16"/>
@@ -8162,14 +8164,14 @@
       <c r="EB59" s="16"/>
     </row>
     <row r="60" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G60" s="61"/>
-      <c r="O60" s="104"/>
-      <c r="P60" s="97"/>
-      <c r="Q60" s="96"/>
-      <c r="R60" s="96"/>
+      <c r="G60" s="56"/>
+      <c r="O60" s="96"/>
+      <c r="P60" s="89"/>
+      <c r="Q60" s="88"/>
+      <c r="R60" s="88"/>
       <c r="S60" s="16"/>
       <c r="T60" s="16"/>
       <c r="U60" s="16"/>
@@ -8286,11 +8288,11 @@
       <c r="EB60" s="16"/>
     </row>
     <row r="61" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G61" s="61"/>
-      <c r="O61" s="104"/>
-      <c r="P61" s="97"/>
-      <c r="Q61" s="96"/>
-      <c r="R61" s="96"/>
+      <c r="G61" s="56"/>
+      <c r="O61" s="96"/>
+      <c r="P61" s="89"/>
+      <c r="Q61" s="88"/>
+      <c r="R61" s="88"/>
       <c r="S61" s="16"/>
       <c r="T61" s="16"/>
       <c r="U61" s="16"/>
@@ -8407,11 +8409,11 @@
       <c r="EB61" s="16"/>
     </row>
     <row r="62" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G62" s="61"/>
-      <c r="O62" s="104"/>
-      <c r="P62" s="97"/>
-      <c r="Q62" s="96"/>
-      <c r="R62" s="96"/>
+      <c r="G62" s="56"/>
+      <c r="O62" s="96"/>
+      <c r="P62" s="89"/>
+      <c r="Q62" s="88"/>
+      <c r="R62" s="88"/>
       <c r="S62" s="16"/>
       <c r="T62" s="16"/>
       <c r="U62" s="16"/>
@@ -8528,14 +8530,14 @@
       <c r="EB62" s="16"/>
     </row>
     <row r="63" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A63" s="75" t="s">
+      <c r="A63" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="G63" s="61"/>
-      <c r="O63" s="104"/>
-      <c r="P63" s="97"/>
-      <c r="Q63" s="96"/>
-      <c r="R63" s="96"/>
+      <c r="G63" s="56"/>
+      <c r="O63" s="96"/>
+      <c r="P63" s="89"/>
+      <c r="Q63" s="88"/>
+      <c r="R63" s="88"/>
       <c r="S63" s="16"/>
       <c r="T63" s="16"/>
       <c r="U63" s="16"/>
@@ -8652,14 +8654,14 @@
       <c r="EB63" s="16"/>
     </row>
     <row r="64" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A64" s="45" t="s">
+      <c r="A64" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G64" s="61"/>
-      <c r="O64" s="104"/>
-      <c r="P64" s="97"/>
-      <c r="Q64" s="96"/>
-      <c r="R64" s="96"/>
+      <c r="G64" s="56"/>
+      <c r="O64" s="96"/>
+      <c r="P64" s="89"/>
+      <c r="Q64" s="88"/>
+      <c r="R64" s="88"/>
       <c r="S64" s="16"/>
       <c r="T64" s="16"/>
       <c r="U64" s="16"/>
@@ -8776,11 +8778,11 @@
       <c r="EB64" s="16"/>
     </row>
     <row r="65" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G65" s="61"/>
-      <c r="O65" s="104"/>
-      <c r="P65" s="97"/>
-      <c r="Q65" s="96"/>
-      <c r="R65" s="96"/>
+      <c r="G65" s="56"/>
+      <c r="O65" s="96"/>
+      <c r="P65" s="89"/>
+      <c r="Q65" s="88"/>
+      <c r="R65" s="88"/>
       <c r="S65" s="16"/>
       <c r="T65" s="16"/>
       <c r="U65" s="16"/>
@@ -8897,8 +8899,8 @@
       <c r="EB65" s="16"/>
     </row>
     <row r="66" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G66" s="61"/>
-      <c r="P66" s="37"/>
+      <c r="G66" s="56"/>
+      <c r="P66" s="34"/>
       <c r="Q66" s="16"/>
       <c r="R66" s="16"/>
       <c r="S66" s="16"/>
@@ -9017,11 +9019,11 @@
       <c r="EB66" s="16"/>
     </row>
     <row r="67" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A67" s="75" t="s">
+      <c r="A67" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G67" s="61"/>
-      <c r="P67" s="37"/>
+      <c r="G67" s="56"/>
+      <c r="P67" s="34"/>
       <c r="Q67" s="16"/>
       <c r="R67" s="16"/>
       <c r="S67" s="16"/>
@@ -9140,11 +9142,11 @@
       <c r="EB67" s="16"/>
     </row>
     <row r="68" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A68" s="45" t="s">
+      <c r="A68" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G68" s="61"/>
-      <c r="P68" s="37"/>
+      <c r="G68" s="56"/>
+      <c r="P68" s="34"/>
       <c r="Q68" s="16"/>
       <c r="R68" s="16"/>
       <c r="S68" s="16"/>
@@ -9263,8 +9265,8 @@
       <c r="EB68" s="16"/>
     </row>
     <row r="69" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G69" s="61"/>
-      <c r="P69" s="37"/>
+      <c r="G69" s="56"/>
+      <c r="P69" s="34"/>
       <c r="Q69" s="16"/>
       <c r="R69" s="16"/>
       <c r="S69" s="16"/>
@@ -9383,11 +9385,11 @@
       <c r="EB69" s="16"/>
     </row>
     <row r="70" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A70" s="45" t="s">
+      <c r="A70" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G70" s="61"/>
-      <c r="P70" s="37"/>
+      <c r="G70" s="56"/>
+      <c r="P70" s="34"/>
       <c r="Q70" s="16"/>
       <c r="R70" s="16"/>
       <c r="S70" s="16"/>
@@ -9506,11 +9508,11 @@
       <c r="EB70" s="16"/>
     </row>
     <row r="71" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A71" s="75" t="s">
+      <c r="A71" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="G71" s="61"/>
-      <c r="P71" s="37"/>
+      <c r="G71" s="56"/>
+      <c r="P71" s="34"/>
       <c r="Q71" s="16"/>
       <c r="R71" s="16"/>
       <c r="S71" s="16"/>
@@ -9629,11 +9631,11 @@
       <c r="EB71" s="16"/>
     </row>
     <row r="72" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A72" s="45" t="s">
+      <c r="A72" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="G72" s="61"/>
-      <c r="P72" s="37"/>
+      <c r="G72" s="56"/>
+      <c r="P72" s="34"/>
       <c r="Q72" s="16"/>
       <c r="R72" s="16"/>
       <c r="S72" s="16"/>
@@ -9752,11 +9754,11 @@
       <c r="EB72" s="16"/>
     </row>
     <row r="73" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A73" s="45" t="s">
+      <c r="A73" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="G73" s="61"/>
-      <c r="P73" s="37"/>
+      <c r="G73" s="56"/>
+      <c r="P73" s="34"/>
       <c r="Q73" s="16"/>
       <c r="R73" s="16"/>
       <c r="S73" s="16"/>
@@ -9875,8 +9877,8 @@
       <c r="EB73" s="16"/>
     </row>
     <row r="74" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G74" s="61"/>
-      <c r="P74" s="37"/>
+      <c r="G74" s="56"/>
+      <c r="P74" s="34"/>
       <c r="Q74" s="16"/>
       <c r="R74" s="16"/>
       <c r="S74" s="16"/>
@@ -9995,448 +9997,448 @@
       <c r="EB74" s="16"/>
     </row>
     <row r="75" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A75" s="45" t="s">
+      <c r="A75" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G75" s="61"/>
+      <c r="G75" s="56"/>
     </row>
     <row r="76" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G76" s="61"/>
+      <c r="G76" s="56"/>
     </row>
     <row r="77" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A77" s="45" t="s">
+      <c r="A77" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G77" s="61"/>
-      <c r="P77" s="67" t="s">
+      <c r="G77" s="56"/>
+      <c r="P77" s="61" t="s">
         <v>56</v>
       </c>
       <c r="Z77" s="15"/>
     </row>
     <row r="78" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A78" s="45" t="s">
+      <c r="A78" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G78" s="61"/>
-      <c r="P78" s="45" t="s">
+      <c r="G78" s="56"/>
+      <c r="P78" s="40" t="s">
         <v>38</v>
       </c>
       <c r="Z78" s="15"/>
     </row>
     <row r="79" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="A79" s="45" t="s">
+      <c r="A79" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G79" s="61"/>
-      <c r="P79" s="45" t="s">
+      <c r="G79" s="56"/>
+      <c r="P79" s="40" t="s">
         <v>37</v>
       </c>
       <c r="Z79" s="15"/>
     </row>
     <row r="80" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="G80" s="61"/>
+      <c r="G80" s="56"/>
       <c r="Z80" s="15"/>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G81" s="61"/>
+      <c r="G81" s="56"/>
       <c r="Z81" s="15"/>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G82" s="61"/>
+      <c r="G82" s="56"/>
       <c r="Z82" s="15"/>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A83" s="74" t="s">
+      <c r="A83" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="P83" s="45" t="s">
+      <c r="P83" s="40" t="s">
         <v>39</v>
       </c>
       <c r="Z83" s="15"/>
     </row>
     <row r="84" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="75" t="s">
+      <c r="A84" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="G84" s="34" t="s">
+      <c r="G84" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="L84" s="36" t="s">
+      <c r="L84" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="M84" s="35" t="s">
+      <c r="M84" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="P84" s="45" t="s">
+      <c r="P84" s="40" t="s">
         <v>42</v>
       </c>
       <c r="Z84" s="15"/>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A85" s="45" t="s">
+      <c r="A85" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B85" s="30"/>
-      <c r="C85" s="30"/>
-      <c r="G85" s="34"/>
-      <c r="L85" s="36"/>
-      <c r="M85" s="35"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="G85" s="31"/>
+      <c r="L85" s="33"/>
+      <c r="M85" s="32"/>
       <c r="Z85" s="15"/>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A86" s="45" t="s">
+      <c r="A86" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30"/>
-      <c r="G86" s="34"/>
-      <c r="L86" s="36"/>
-      <c r="M86" s="35"/>
-      <c r="P86" s="45" t="s">
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
+      <c r="G86" s="31"/>
+      <c r="L86" s="33"/>
+      <c r="M86" s="32"/>
+      <c r="P86" s="40" t="s">
         <v>34</v>
       </c>
       <c r="Z86" s="15"/>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A87" s="45" t="s">
+      <c r="A87" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D87" s="30"/>
-      <c r="G87" s="34"/>
-      <c r="L87" s="36"/>
-      <c r="M87" s="35"/>
-      <c r="P87" s="45" t="s">
+      <c r="D87" s="29"/>
+      <c r="G87" s="31"/>
+      <c r="L87" s="33"/>
+      <c r="M87" s="32"/>
+      <c r="P87" s="40" t="s">
         <v>35</v>
       </c>
       <c r="Z87" s="15"/>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A88" s="45" t="s">
+      <c r="A88" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="G88" s="34"/>
-      <c r="L88" s="36"/>
-      <c r="M88" s="35"/>
-      <c r="P88" s="45" t="s">
+      <c r="G88" s="31"/>
+      <c r="L88" s="33"/>
+      <c r="M88" s="32"/>
+      <c r="P88" s="40" t="s">
         <v>36</v>
       </c>
       <c r="Z88" s="15"/>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A89" s="45" t="s">
+      <c r="A89" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="F89" s="30"/>
-      <c r="G89" s="34"/>
-      <c r="H89" s="30"/>
-      <c r="L89" s="36"/>
-      <c r="M89" s="35"/>
+      <c r="F89" s="29"/>
+      <c r="G89" s="31"/>
+      <c r="H89" s="29"/>
+      <c r="L89" s="33"/>
+      <c r="M89" s="32"/>
       <c r="Z89" s="15"/>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G90" s="34"/>
-      <c r="L90" s="36"/>
-      <c r="M90" s="35"/>
-      <c r="P90" s="75" t="s">
+      <c r="G90" s="31"/>
+      <c r="L90" s="33"/>
+      <c r="M90" s="32"/>
+      <c r="P90" s="69" t="s">
         <v>9</v>
       </c>
       <c r="Z90" s="15"/>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A91" s="75" t="s">
+      <c r="A91" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="E91" s="30"/>
-      <c r="G91" s="34"/>
-      <c r="L91" s="36"/>
-      <c r="M91" s="35"/>
-      <c r="P91" s="45" t="s">
+      <c r="E91" s="29"/>
+      <c r="G91" s="31"/>
+      <c r="L91" s="33"/>
+      <c r="M91" s="32"/>
+      <c r="P91" s="40" t="s">
         <v>31</v>
       </c>
       <c r="Z91" s="15"/>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A92" s="45" t="s">
+      <c r="A92" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="F92" s="30"/>
-      <c r="G92" s="34"/>
-      <c r="L92" s="36"/>
-      <c r="M92" s="35"/>
-      <c r="P92" s="45" t="s">
+      <c r="F92" s="29"/>
+      <c r="G92" s="31"/>
+      <c r="L92" s="33"/>
+      <c r="M92" s="32"/>
+      <c r="P92" s="40" t="s">
         <v>32</v>
       </c>
       <c r="Z92" s="15"/>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A93" s="45" t="s">
+      <c r="A93" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F93" s="30"/>
-      <c r="G93" s="34"/>
-      <c r="L93" s="36"/>
-      <c r="M93" s="35"/>
-      <c r="P93" s="45" t="s">
+      <c r="F93" s="29"/>
+      <c r="G93" s="31"/>
+      <c r="L93" s="33"/>
+      <c r="M93" s="32"/>
+      <c r="P93" s="40" t="s">
         <v>33</v>
       </c>
       <c r="Z93" s="15"/>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A94" s="45" t="s">
+      <c r="A94" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="F94" s="30"/>
-      <c r="G94" s="34"/>
-      <c r="L94" s="36"/>
-      <c r="M94" s="35"/>
+      <c r="F94" s="29"/>
+      <c r="G94" s="31"/>
+      <c r="L94" s="33"/>
+      <c r="M94" s="32"/>
       <c r="Z94" s="15"/>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G95" s="34"/>
-      <c r="L95" s="36"/>
-      <c r="M95" s="35"/>
-      <c r="P95" s="75" t="s">
+      <c r="G95" s="31"/>
+      <c r="L95" s="33"/>
+      <c r="M95" s="32"/>
+      <c r="P95" s="69" t="s">
         <v>19</v>
       </c>
       <c r="Z95" s="15"/>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A96" s="75" t="s">
+      <c r="A96" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="G96" s="34"/>
-      <c r="L96" s="36"/>
-      <c r="M96" s="35"/>
-      <c r="P96" s="45" t="s">
+      <c r="G96" s="31"/>
+      <c r="L96" s="33"/>
+      <c r="M96" s="32"/>
+      <c r="P96" s="40" t="s">
         <v>31</v>
       </c>
       <c r="Z96" s="15"/>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A97" s="45" t="s">
+      <c r="A97" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="30"/>
-      <c r="G97" s="34"/>
-      <c r="L97" s="36"/>
-      <c r="M97" s="35"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="31"/>
+      <c r="L97" s="33"/>
+      <c r="M97" s="32"/>
       <c r="Z97" s="15"/>
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A98" s="45" t="s">
+      <c r="A98" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G98" s="34"/>
-      <c r="L98" s="36"/>
-      <c r="M98" s="35"/>
+      <c r="G98" s="31"/>
+      <c r="L98" s="33"/>
+      <c r="M98" s="32"/>
       <c r="Z98" s="15"/>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A99" s="45" t="s">
+      <c r="A99" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="B99" s="30"/>
-      <c r="G99" s="34"/>
+      <c r="B99" s="29"/>
+      <c r="G99" s="31"/>
       <c r="H99" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="L99" s="36"/>
-      <c r="M99" s="35"/>
-      <c r="P99" s="75" t="s">
+      <c r="L99" s="33"/>
+      <c r="M99" s="32"/>
+      <c r="P99" s="69" t="s">
         <v>12</v>
       </c>
       <c r="Z99" s="15"/>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A100" s="45" t="s">
+      <c r="A100" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="B100" s="30"/>
-      <c r="G100" s="34"/>
-      <c r="H100" s="30"/>
-      <c r="L100" s="36"/>
-      <c r="M100" s="35"/>
-      <c r="P100" s="45" t="s">
+      <c r="B100" s="29"/>
+      <c r="G100" s="31"/>
+      <c r="H100" s="29"/>
+      <c r="L100" s="33"/>
+      <c r="M100" s="32"/>
+      <c r="P100" s="40" t="s">
         <v>31</v>
       </c>
       <c r="Z100" s="15"/>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A101" s="45" t="s">
+      <c r="A101" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="C101" s="30"/>
-      <c r="D101" s="30"/>
-      <c r="G101" s="34"/>
-      <c r="I101" s="30"/>
-      <c r="L101" s="36"/>
-      <c r="M101" s="35"/>
+      <c r="C101" s="29"/>
+      <c r="D101" s="29"/>
+      <c r="G101" s="31"/>
+      <c r="I101" s="29"/>
+      <c r="L101" s="33"/>
+      <c r="M101" s="32"/>
       <c r="Z101" s="15"/>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A102" s="45" t="s">
+      <c r="A102" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B102" s="30"/>
-      <c r="C102" s="30"/>
-      <c r="D102" s="30"/>
-      <c r="E102" s="30"/>
-      <c r="F102" s="30"/>
-      <c r="G102" s="34"/>
-      <c r="H102" s="30"/>
-      <c r="I102" s="30"/>
-      <c r="J102" s="30"/>
-      <c r="L102" s="36"/>
-      <c r="M102" s="35"/>
+      <c r="B102" s="29"/>
+      <c r="C102" s="29"/>
+      <c r="D102" s="29"/>
+      <c r="E102" s="29"/>
+      <c r="F102" s="29"/>
+      <c r="G102" s="31"/>
+      <c r="H102" s="29"/>
+      <c r="I102" s="29"/>
+      <c r="J102" s="29"/>
+      <c r="L102" s="33"/>
+      <c r="M102" s="32"/>
       <c r="Z102" s="15"/>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A103" s="45" t="s">
+      <c r="A103" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="G103" s="34"/>
-      <c r="H103" s="30"/>
-      <c r="L103" s="36"/>
-      <c r="M103" s="35"/>
-      <c r="P103" s="75" t="s">
+      <c r="G103" s="31"/>
+      <c r="H103" s="29"/>
+      <c r="L103" s="33"/>
+      <c r="M103" s="32"/>
+      <c r="P103" s="69" t="s">
         <v>15</v>
       </c>
       <c r="Z103" s="15"/>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A104" s="45" t="s">
+      <c r="A104" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="G104" s="34"/>
-      <c r="I104" s="30"/>
-      <c r="L104" s="36"/>
-      <c r="M104" s="35"/>
-      <c r="P104" s="45" t="s">
+      <c r="G104" s="31"/>
+      <c r="I104" s="29"/>
+      <c r="L104" s="33"/>
+      <c r="M104" s="32"/>
+      <c r="P104" s="40" t="s">
         <v>31</v>
       </c>
       <c r="Z104" s="15"/>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G105" s="34"/>
-      <c r="L105" s="36"/>
-      <c r="M105" s="35"/>
+      <c r="G105" s="31"/>
+      <c r="L105" s="33"/>
+      <c r="M105" s="32"/>
       <c r="Z105" s="15"/>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A106" s="76" t="s">
+      <c r="A106" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="G106" s="34"/>
-      <c r="L106" s="36"/>
-      <c r="M106" s="35"/>
-      <c r="P106" s="45" t="s">
+      <c r="G106" s="31"/>
+      <c r="L106" s="33"/>
+      <c r="M106" s="32"/>
+      <c r="P106" s="40" t="s">
         <v>25</v>
       </c>
       <c r="Z106" s="15"/>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A107" s="77" t="s">
+      <c r="A107" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="B107" s="30"/>
-      <c r="G107" s="34"/>
-      <c r="L107" s="36"/>
-      <c r="M107" s="35"/>
-      <c r="P107" s="75" t="s">
+      <c r="B107" s="29"/>
+      <c r="G107" s="31"/>
+      <c r="L107" s="33"/>
+      <c r="M107" s="32"/>
+      <c r="P107" s="69" t="s">
         <v>16</v>
       </c>
       <c r="Z107" s="15"/>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A108" s="77" t="s">
+      <c r="A108" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="D108" s="30"/>
-      <c r="G108" s="34"/>
-      <c r="H108" s="30"/>
-      <c r="L108" s="36"/>
-      <c r="M108" s="35"/>
-      <c r="P108" s="45" t="s">
+      <c r="D108" s="29"/>
+      <c r="G108" s="31"/>
+      <c r="H108" s="29"/>
+      <c r="L108" s="33"/>
+      <c r="M108" s="32"/>
+      <c r="P108" s="40" t="s">
         <v>26</v>
       </c>
       <c r="Z108" s="15"/>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A109" s="77" t="s">
+      <c r="A109" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="G109" s="34"/>
-      <c r="I109" s="30"/>
-      <c r="J109" s="30"/>
-      <c r="L109" s="36"/>
-      <c r="M109" s="35"/>
-      <c r="P109" s="45" t="s">
+      <c r="G109" s="31"/>
+      <c r="I109" s="29"/>
+      <c r="J109" s="29"/>
+      <c r="L109" s="33"/>
+      <c r="M109" s="32"/>
+      <c r="P109" s="40" t="s">
         <v>27</v>
       </c>
       <c r="Z109" s="15"/>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A110" s="77" t="s">
+      <c r="A110" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="G110" s="34"/>
-      <c r="J110" s="30"/>
-      <c r="L110" s="36"/>
-      <c r="M110" s="35"/>
+      <c r="G110" s="31"/>
+      <c r="J110" s="29"/>
+      <c r="L110" s="33"/>
+      <c r="M110" s="32"/>
       <c r="Z110" s="15"/>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A111" s="77" t="s">
+      <c r="A111" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="G111" s="34"/>
-      <c r="I111" s="30"/>
-      <c r="L111" s="36"/>
-      <c r="M111" s="35"/>
-      <c r="P111" s="45" t="s">
+      <c r="G111" s="31"/>
+      <c r="I111" s="29"/>
+      <c r="L111" s="33"/>
+      <c r="M111" s="32"/>
+      <c r="P111" s="40" t="s">
         <v>28</v>
       </c>
       <c r="Z111" s="15"/>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A112" s="77" t="s">
+      <c r="A112" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="G112" s="34"/>
-      <c r="I112" s="30"/>
-      <c r="L112" s="36"/>
-      <c r="M112" s="35"/>
+      <c r="G112" s="31"/>
+      <c r="I112" s="29"/>
+      <c r="L112" s="33"/>
+      <c r="M112" s="32"/>
       <c r="Z112" s="15"/>
     </row>
     <row r="113" spans="16:26" x14ac:dyDescent="0.25">
-      <c r="P113" s="45" t="s">
+      <c r="P113" s="40" t="s">
         <v>29</v>
       </c>
       <c r="Z113" s="15"/>
     </row>
     <row r="114" spans="16:26" x14ac:dyDescent="0.25">
-      <c r="P114" s="45" t="s">
+      <c r="P114" s="40" t="s">
         <v>30</v>
       </c>
       <c r="Z114" s="15"/>
     </row>
     <row r="115" spans="16:26" x14ac:dyDescent="0.25">
-      <c r="P115" s="45" t="s">
+      <c r="P115" s="40" t="s">
         <v>24</v>
       </c>
       <c r="Z115" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="Q38:AB41"/>
+    <mergeCell ref="B38:M41"/>
     <mergeCell ref="P1:P3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="V4:V36"/>
     <mergeCell ref="AA4:AA36"/>
     <mergeCell ref="AB4:AB36"/>
-    <mergeCell ref="Q38:AB41"/>
-    <mergeCell ref="B38:M41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10448,7 +10450,7 @@
   <dimension ref="A2:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10525,6 +10527,7 @@
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="B10" s="3"/>
       <c r="G10" t="s">
         <v>35</v>
       </c>
@@ -10609,11 +10612,13 @@
       <c r="A23" t="s">
         <v>13</v>
       </c>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
+      <c r="B24" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">

</xml_diff>